<commit_message>
fix: agendamento friday e new xlsx
</commit_message>
<xml_diff>
--- a/data/Links BI Vendedores.xlsx
+++ b/data/Links BI Vendedores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Matriz\Pojetos_Geral\Projeto_bruno\apoio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF1D150-E4D5-4ABC-8355-969F47083D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6ED66C-CDB6-467B-B414-D658677032E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E0E5992F-4932-4BF3-AAB7-E3FBA91C53F9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Nome Vendedor</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Link BI</t>
   </si>
   <si>
-    <t>https://app.powerbi.com/reportEmbed?reportId=89c95e86-355f-49d4-8f08-3f0789fcc3fb&amp;autoAuth=true&amp;ctid=588dc949-c01b-4573-bbb3-dd903341a9c4</t>
-  </si>
-  <si>
-    <t>https://app.powerbi.com/reportEmbed?reportId=f533b7f1-a49f-40e1-b832-a7df86d71765&amp;autoAuth=true&amp;ctid=588dc949-c01b-4573-bbb3-dd903341a9c4</t>
-  </si>
-  <si>
     <t>exportsales2@bmgfoods.com.br</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Jhazz Argüello</t>
   </si>
   <si>
-    <t>https://app.powerbi.com/reportEmbed?reportId=781b746a-9b71-46c9-affa-670ea1e4e4bc&amp;autoAuth=true&amp;ctid=588dc949-c01b-4573-bbb3-dd903341a9c4</t>
-  </si>
-  <si>
     <t>alvaro@frigoconcepcion.com.py</t>
   </si>
   <si>
@@ -75,9 +66,6 @@
     <t>Alvaro D'Abbisogno</t>
   </si>
   <si>
-    <t>https://app.powerbi.com/reportEmbed?reportId=0fa58f18-8071-44ca-9045-fd21371f2a21&amp;autoAuth=true&amp;ctid=588dc949-c01b-4573-bbb3-dd903341a9c4</t>
-  </si>
-  <si>
     <t>exportsales1@bmgfoods.com.br</t>
   </si>
   <si>
@@ -87,9 +75,6 @@
     <t>Maria José Reynot</t>
   </si>
   <si>
-    <t>https://app.powerbi.com/reportEmbed?reportId=6cbce9c9-0e27-4a80-bac4-bcf178fe35c4&amp;autoAuth=true&amp;ctid=588dc949-c01b-4573-bbb3-dd903341a9c4</t>
-  </si>
-  <si>
     <t>andre@frigoconcepcion.com.py</t>
   </si>
   <si>
@@ -99,9 +84,6 @@
     <t>Andre Candia</t>
   </si>
   <si>
-    <t>https://app.powerbi.com/reportEmbed?reportId=cb46b153-6673-47bf-b239-0ac90577b03a&amp;autoAuth=true&amp;ctid=588dc949-c01b-4573-bbb3-dd903341a9c4</t>
-  </si>
-  <si>
     <t>marcus@frigoconcepcion.com.py</t>
   </si>
   <si>
@@ -111,9 +93,6 @@
     <t>Marcus Mendes</t>
   </si>
   <si>
-    <t>https://app.powerbi.com/reportEmbed?reportId=54d707ed-d121-4d63-9c46-6d6215cdab73&amp;autoAuth=true&amp;ctid=588dc949-c01b-4573-bbb3-dd903341a9c4</t>
-  </si>
-  <si>
     <t>cmfred@frigoconcepcion.com.py</t>
   </si>
   <si>
@@ -132,17 +111,43 @@
     <t>export.gp@bmgfoods.com.br</t>
   </si>
   <si>
-    <t>https://app.powerbi.com/reportEmbed?reportId=aa95f991-7723-4c7e-b082-8a884cbbaeeb&amp;autoAuth=true&amp;ctid=588dc949-c01b-4573-bbb3-dd903341a9c4</t>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiYzhmZjFiZmItZWExYS00NzJjLWEyOTYtYjYxZGIxMzYyYWUxIiwidCI6IjU4OGRjOTQ5LWMwMWItNDU3My1iYmIzLWRkOTAzMzQxYTljNCJ9</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiMmJkZWJmOTMtMWJjMS00YmEyLWJmNDgtYjgyMzA5MTFkZmI0IiwidCI6IjU4OGRjOTQ5LWMwMWItNDU3My1iYmIzLWRkOTAzMzQxYTljNCJ9</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiYTllMDAwMWUtNmFiYi00MTFmLWIyYWQtOWJkZDgxM2VhNGNjIiwidCI6IjU4OGRjOTQ5LWMwMWItNDU3My1iYmIzLWRkOTAzMzQxYTljNCJ9</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiZTg5MjU1OTAtZWZkMC00MDA2LWJhMTYtMzFkZThkNjE1NzhkIiwidCI6IjU4OGRjOTQ5LWMwMWItNDU3My1iYmIzLWRkOTAzMzQxYTljNCJ9</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiNjUzNDcxMTItNzE0OC00MmM0LWI2NmItMWNhZWZlNWUwYWZmIiwidCI6IjU4OGRjOTQ5LWMwMWItNDU3My1iYmIzLWRkOTAzMzQxYTljNCJ9</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiMjE4ZGYxYzktMzEwZi00NTIwLWIxMjQtZTUwZTgxNDZiMWU5IiwidCI6IjU4OGRjOTQ5LWMwMWItNDU3My1iYmIzLWRkOTAzMzQxYTljNCJ9</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiYWIwYzQwNjMtZGViNy00NmMzLTk2YjAtM2ZhNDQ1MTQ2MjkxIiwidCI6IjU4OGRjOTQ5LWMwMWItNDU3My1iYmIzLWRkOTAzMzQxYTljNCJ9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,13 +170,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,7 +495,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,109 +530,118 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{F95D4D75-FA1C-4F5B-845D-470BBA15A554}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{6667EA34-6578-4CB9-87DF-99631B26ED76}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{93299E40-BF12-4AB2-9869-1DEEF5ACDEE2}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{81B62792-49DC-4FEE-85BA-A36F82A3F86A}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{640414F5-8157-480C-A6A3-5627AFE8B435}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{1F895710-3FA3-4D08-BF16-580722124F10}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{276F3DC5-9D24-4D1F-A53E-C6D97BF75E46}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>